<commit_message>
final, fix getattribute error
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,6 +458,339 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Linh Đàm</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Botanix Cafe</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>105.8251937</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>20.9656864</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>cà phê</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>4,4</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>(165)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Linh Đàm</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Cộng Cà Phê</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>105.825746</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>20.9634174</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>cà phê</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>4,0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>(1.281)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Linh Đàm</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Cafe Chouchi</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>105.8226406</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>20.9633296</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>cà phê</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>4,2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>(443)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Linh Đàm</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Quán The Coffee House</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>105.8229694</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>20.9634459</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>cà phê</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>4,4</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>(535)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Linh Đàm</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>House of Cha Coffee</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>105.8238937</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>20.962895</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>cà phê</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>4,5</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>(26)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Linh Đàm</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Highlands Coffee</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>105.8254817</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>20.9638615</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>cà phê</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>4,2</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>(867)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Linh Đàm</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Laika Cafe Linh Đàm</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>105.8256359</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>20.9653021</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>cà phê</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>4,2</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>(239)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Linh Đàm</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Forli Coffee &amp; Tea</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>105.8272274</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>20.9712171</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>cà phê</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>4,7</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>(50)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Linh Đàm</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Milano Coffee</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>105.8251697</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>20.966328</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>cà phê</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>4,2</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>(132)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>